<commit_message>
Cluster por cada año
</commit_message>
<xml_diff>
--- a/NacimientosDesglose.xlsx
+++ b/NacimientosDesglose.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10409"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alegomez/Documents/UVG/Cuarto Año/Primer Semestre/Mineria/Proyecto1/Proyecto1-MD/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\UNIVERSIDAD\7MO SEMESTRE\MINERIA DE DATOS\Proyecto1-MD\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{952B261F-426F-C147-9FCF-A91B264B2490}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71C03C6C-7020-4D23-8D1D-050116EE386A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" xr2:uid="{A65F4AA3-2E4A-8040-8E4B-2C73C7A3E010}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{A65F4AA3-2E4A-8040-8E4B-2C73C7A3E010}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -39,9 +39,6 @@
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="320" uniqueCount="32">
   <si>
     <t>Año</t>
-  </si>
-  <si>
-    <t>Departamento de residencia</t>
   </si>
   <si>
     <t>Total</t>
@@ -133,13 +130,16 @@
   <si>
     <t xml:space="preserve"> -</t>
   </si>
+  <si>
+    <t>Departamento</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="41" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="164" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -207,10 +207,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="41" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="41" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -231,7 +231,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -530,45 +530,45 @@
   <dimension ref="A1:G313"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1:G1"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.83203125" style="1"/>
-    <col min="2" max="2" width="25.1640625" style="2" customWidth="1"/>
-    <col min="3" max="7" width="10.83203125" style="1"/>
+    <col min="1" max="1" width="10.875" style="1"/>
+    <col min="2" max="2" width="25.125" style="2" customWidth="1"/>
+    <col min="3" max="7" width="10.875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="28" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="E1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="E1" s="3" t="s">
+      <c r="F1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="G1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="G1" s="3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>2009</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C2" s="1">
         <v>58906</v>
@@ -586,12 +586,12 @@
         <v>29022</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>2009</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C3" s="1">
         <v>3814</v>
@@ -609,12 +609,12 @@
         <v>1865</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>2009</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C4" s="1">
         <v>6708</v>
@@ -632,12 +632,12 @@
         <v>3273</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>2009</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C5" s="1">
         <v>14482</v>
@@ -655,12 +655,12 @@
         <v>7069</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>2009</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C6" s="1">
         <v>14552</v>
@@ -678,12 +678,12 @@
         <v>7097</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>2009</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C7" s="1">
         <v>8181</v>
@@ -701,12 +701,12 @@
         <v>4016</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>2009</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C8" s="1">
         <v>9511</v>
@@ -724,12 +724,12 @@
         <v>4673</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>2009</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C9" s="1">
         <v>11410</v>
@@ -747,12 +747,12 @@
         <v>5618</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>2009</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C10" s="1">
         <v>18653</v>
@@ -770,12 +770,12 @@
         <v>9262</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>2009</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C11" s="1">
         <v>12771</v>
@@ -793,12 +793,12 @@
         <v>6228</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>2009</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C12" s="1">
         <v>7297</v>
@@ -816,12 +816,12 @@
         <v>3541</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>2009</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C13" s="1">
         <v>27590</v>
@@ -839,12 +839,12 @@
         <v>13536</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>2009</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C14" s="1">
         <v>32782</v>
@@ -862,12 +862,12 @@
         <v>16230</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>2009</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C15" s="1">
         <v>26849</v>
@@ -885,12 +885,12 @@
         <v>13155</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>2009</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C16" s="1">
         <v>7218</v>
@@ -908,12 +908,12 @@
         <v>3572</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>2009</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C17" s="1">
         <v>32925</v>
@@ -931,12 +931,12 @@
         <v>16328</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <v>2009</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C18" s="1">
         <v>13632</v>
@@ -954,12 +954,12 @@
         <v>6695</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <v>2009</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C19" s="1">
         <v>8956</v>
@@ -977,12 +977,12 @@
         <v>4392</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <v>2009</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C20" s="1">
         <v>5626</v>
@@ -1000,12 +1000,12 @@
         <v>2725</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <v>2009</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C21" s="1">
         <v>10181</v>
@@ -1023,12 +1023,12 @@
         <v>4925</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
         <v>2009</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C22" s="1">
         <v>8270</v>
@@ -1046,12 +1046,12 @@
         <v>4064</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
         <v>2009</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C23" s="1">
         <v>10809</v>
@@ -1069,12 +1069,12 @@
         <v>5244</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
         <v>2009</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C24" s="1">
         <v>129</v>
@@ -1092,12 +1092,12 @@
         <v>54</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
         <v>2009</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C25" s="1">
         <v>376</v>
@@ -1115,12 +1115,12 @@
         <v>181</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
         <v>2010</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C26" s="1">
         <f>E26-D26</f>
@@ -1139,15 +1139,15 @@
         <v>29137</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
         <v>2010</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C27" s="1">
-        <f t="shared" ref="C27:C73" si="0">E27-D27</f>
+        <f t="shared" ref="C27:C72" si="0">E27-D27</f>
         <v>3761</v>
       </c>
       <c r="D27" s="1">
@@ -1163,12 +1163,12 @@
         <v>1845</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
         <v>2010</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C28" s="1">
         <f t="shared" si="0"/>
@@ -1187,12 +1187,12 @@
         <v>3248</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
         <v>2010</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C29" s="1">
         <f t="shared" si="0"/>
@@ -1211,12 +1211,12 @@
         <v>7489</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
         <v>2010</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C30" s="1">
         <f t="shared" si="0"/>
@@ -1235,12 +1235,12 @@
         <v>7028</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" s="1">
         <v>2010</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C31" s="1">
         <f t="shared" si="0"/>
@@ -1259,12 +1259,12 @@
         <v>3987</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" s="1">
         <v>2010</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C32" s="1">
         <f t="shared" si="0"/>
@@ -1283,12 +1283,12 @@
         <v>4620</v>
       </c>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" s="1">
         <v>2010</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C33" s="1">
         <f t="shared" si="0"/>
@@ -1307,12 +1307,12 @@
         <v>5720</v>
       </c>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34" s="1">
         <v>2010</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C34" s="1">
         <f t="shared" si="0"/>
@@ -1331,12 +1331,12 @@
         <v>9417</v>
       </c>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" s="1">
         <v>2010</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C35" s="1">
         <f t="shared" si="0"/>
@@ -1355,12 +1355,12 @@
         <v>6336</v>
       </c>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" s="1">
         <v>2010</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C36" s="1">
         <f t="shared" si="0"/>
@@ -1379,12 +1379,12 @@
         <v>3671</v>
       </c>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37" s="1">
         <v>2010</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C37" s="1">
         <f t="shared" si="0"/>
@@ -1403,12 +1403,12 @@
         <v>14445</v>
       </c>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A38" s="1">
         <v>2010</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C38" s="1">
         <f t="shared" si="0"/>
@@ -1427,12 +1427,12 @@
         <v>17919</v>
       </c>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A39" s="1">
         <v>2010</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C39" s="1">
         <f t="shared" si="0"/>
@@ -1451,12 +1451,12 @@
         <v>13829</v>
       </c>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A40" s="1">
         <v>2010</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C40" s="1">
         <f t="shared" si="0"/>
@@ -1475,12 +1475,12 @@
         <v>3733</v>
       </c>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A41" s="1">
         <v>2010</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C41" s="1">
         <f t="shared" si="0"/>
@@ -1499,12 +1499,12 @@
         <v>16662</v>
       </c>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A42" s="1">
         <v>2010</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C42" s="1">
         <f t="shared" si="0"/>
@@ -1523,12 +1523,12 @@
         <v>6939</v>
       </c>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A43" s="1">
         <v>2010</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C43" s="1">
         <f t="shared" si="0"/>
@@ -1547,12 +1547,12 @@
         <v>4788</v>
       </c>
     </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A44" s="1">
         <v>2010</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C44" s="1">
         <f t="shared" si="0"/>
@@ -1571,12 +1571,12 @@
         <v>2795</v>
       </c>
     </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A45" s="1">
         <v>2010</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C45" s="1">
         <f t="shared" si="0"/>
@@ -1595,12 +1595,12 @@
         <v>5034</v>
       </c>
     </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A46" s="1">
         <v>2010</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C46" s="1">
         <f t="shared" si="0"/>
@@ -1619,12 +1619,12 @@
         <v>4301</v>
       </c>
     </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A47" s="1">
         <v>2010</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C47" s="1">
         <f t="shared" si="0"/>
@@ -1643,12 +1643,12 @@
         <v>5489</v>
       </c>
     </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A48" s="1">
         <v>2010</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C48" s="1">
         <f t="shared" si="0"/>
@@ -1667,12 +1667,12 @@
         <v>52</v>
       </c>
     </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A49" s="1">
         <v>2010</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C49" s="1">
         <f t="shared" si="0"/>
@@ -1691,12 +1691,12 @@
         <v>68</v>
       </c>
     </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A50" s="1">
         <v>2011</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C50" s="1">
         <f t="shared" si="0"/>
@@ -1715,12 +1715,12 @@
         <v>30431</v>
       </c>
     </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A51" s="1">
         <v>2011</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C51" s="1">
         <f t="shared" si="0"/>
@@ -1739,12 +1739,12 @@
         <v>1974</v>
       </c>
     </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A52" s="1">
         <v>2011</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C52" s="1">
         <f t="shared" si="0"/>
@@ -1763,12 +1763,12 @@
         <v>3391</v>
       </c>
     </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A53" s="1">
         <v>2011</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C53" s="1">
         <f t="shared" si="0"/>
@@ -1787,12 +1787,12 @@
         <v>7526</v>
       </c>
     </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A54" s="1">
         <v>2011</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C54" s="1">
         <f t="shared" si="0"/>
@@ -1811,12 +1811,12 @@
         <v>7764</v>
       </c>
     </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A55" s="1">
         <v>2011</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C55" s="1">
         <f t="shared" si="0"/>
@@ -1835,12 +1835,12 @@
         <v>4433</v>
       </c>
     </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A56" s="1">
         <v>2011</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C56" s="1">
         <f t="shared" si="0"/>
@@ -1859,12 +1859,12 @@
         <v>4739</v>
       </c>
     </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A57" s="1">
         <v>2011</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C57" s="1">
         <f t="shared" si="0"/>
@@ -1883,12 +1883,12 @@
         <v>5765</v>
       </c>
     </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A58" s="1">
         <v>2011</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C58" s="1">
         <f t="shared" si="0"/>
@@ -1907,12 +1907,12 @@
         <v>9753</v>
       </c>
     </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A59" s="1">
         <v>2011</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C59" s="1">
         <f t="shared" si="0"/>
@@ -1931,12 +1931,12 @@
         <v>6811</v>
       </c>
     </row>
-    <row r="60" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A60" s="1">
         <v>2011</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C60" s="1">
         <f t="shared" si="0"/>
@@ -1955,12 +1955,12 @@
         <v>3836</v>
       </c>
     </row>
-    <row r="61" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A61" s="1">
         <v>2011</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C61" s="1">
         <f t="shared" si="0"/>
@@ -1979,12 +1979,12 @@
         <v>14597</v>
       </c>
     </row>
-    <row r="62" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A62" s="1">
         <v>2011</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C62" s="1">
         <f t="shared" si="0"/>
@@ -2003,12 +2003,12 @@
         <v>18280</v>
       </c>
     </row>
-    <row r="63" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A63" s="1">
         <v>2011</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C63" s="1">
         <f t="shared" si="0"/>
@@ -2027,12 +2027,12 @@
         <v>13873</v>
       </c>
     </row>
-    <row r="64" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A64" s="1">
         <v>2011</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C64" s="1">
         <f t="shared" si="0"/>
@@ -2051,12 +2051,12 @@
         <v>3799</v>
       </c>
     </row>
-    <row r="65" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A65" s="1">
         <v>2011</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C65" s="1">
         <f t="shared" si="0"/>
@@ -2075,12 +2075,12 @@
         <v>16427</v>
       </c>
     </row>
-    <row r="66" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A66" s="1">
         <v>2011</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C66" s="1">
         <f t="shared" si="0"/>
@@ -2099,12 +2099,12 @@
         <v>7130</v>
       </c>
     </row>
-    <row r="67" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A67" s="1">
         <v>2011</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C67" s="1">
         <f t="shared" si="0"/>
@@ -2123,12 +2123,12 @@
         <v>5036</v>
       </c>
     </row>
-    <row r="68" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A68" s="1">
         <v>2011</v>
       </c>
       <c r="B68" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C68" s="1">
         <f t="shared" si="0"/>
@@ -2147,12 +2147,12 @@
         <v>2953</v>
       </c>
     </row>
-    <row r="69" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A69" s="1">
         <v>2011</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C69" s="1">
         <f t="shared" si="0"/>
@@ -2171,12 +2171,12 @@
         <v>5304</v>
       </c>
     </row>
-    <row r="70" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A70" s="1">
         <v>2011</v>
       </c>
       <c r="B70" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C70" s="1">
         <f t="shared" si="0"/>
@@ -2195,12 +2195,12 @@
         <v>4402</v>
       </c>
     </row>
-    <row r="71" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A71" s="1">
         <v>2011</v>
       </c>
       <c r="B71" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C71" s="1">
         <f t="shared" si="0"/>
@@ -2219,12 +2219,12 @@
         <v>5598</v>
       </c>
     </row>
-    <row r="72" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A72" s="1">
         <v>2011</v>
       </c>
       <c r="B72" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C72" s="1">
         <f t="shared" si="0"/>
@@ -2243,12 +2243,12 @@
         <v>81</v>
       </c>
     </row>
-    <row r="73" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A73" s="1">
         <v>2011</v>
       </c>
       <c r="B73" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C73" s="1">
         <v>125</v>
@@ -2266,12 +2266,12 @@
         <v>65</v>
       </c>
     </row>
-    <row r="74" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A74" s="1">
         <v>2012</v>
       </c>
       <c r="B74" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C74" s="1">
         <f>E74-D74</f>
@@ -2290,15 +2290,15 @@
         <v>31515</v>
       </c>
     </row>
-    <row r="75" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A75" s="1">
         <v>2012</v>
       </c>
       <c r="B75" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C75" s="1">
-        <f t="shared" ref="C75:C97" si="1">E75-D75</f>
+        <f t="shared" ref="C75:C96" si="1">E75-D75</f>
         <v>4002</v>
       </c>
       <c r="D75" s="1">
@@ -2314,12 +2314,12 @@
         <v>2048</v>
       </c>
     </row>
-    <row r="76" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A76" s="1">
         <v>2012</v>
       </c>
       <c r="B76" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C76" s="1">
         <f t="shared" si="1"/>
@@ -2338,12 +2338,12 @@
         <v>3442</v>
       </c>
     </row>
-    <row r="77" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A77" s="1">
         <v>2012</v>
       </c>
       <c r="B77" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C77" s="1">
         <f t="shared" si="1"/>
@@ -2362,12 +2362,12 @@
         <v>7865</v>
       </c>
     </row>
-    <row r="78" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A78" s="1">
         <v>2012</v>
       </c>
       <c r="B78" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C78" s="1">
         <f t="shared" si="1"/>
@@ -2386,12 +2386,12 @@
         <v>8105</v>
       </c>
     </row>
-    <row r="79" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A79" s="1">
         <v>2012</v>
       </c>
       <c r="B79" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C79" s="1">
         <f t="shared" si="1"/>
@@ -2410,12 +2410,12 @@
         <v>4718</v>
       </c>
     </row>
-    <row r="80" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A80" s="1">
         <v>2012</v>
       </c>
       <c r="B80" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C80" s="1">
         <f t="shared" si="1"/>
@@ -2434,12 +2434,12 @@
         <v>4838</v>
       </c>
     </row>
-    <row r="81" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A81" s="1">
         <v>2012</v>
       </c>
       <c r="B81" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C81" s="1">
         <f t="shared" si="1"/>
@@ -2458,12 +2458,12 @@
         <v>6010</v>
       </c>
     </row>
-    <row r="82" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A82" s="1">
         <v>2012</v>
       </c>
       <c r="B82" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C82" s="1">
         <f t="shared" si="1"/>
@@ -2482,12 +2482,12 @@
         <v>10367</v>
       </c>
     </row>
-    <row r="83" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A83" s="1">
         <v>2012</v>
       </c>
       <c r="B83" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C83" s="1">
         <f t="shared" si="1"/>
@@ -2506,12 +2506,12 @@
         <v>7009</v>
       </c>
     </row>
-    <row r="84" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A84" s="1">
         <v>2012</v>
       </c>
       <c r="B84" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C84" s="1">
         <f t="shared" si="1"/>
@@ -2530,12 +2530,12 @@
         <v>4004</v>
       </c>
     </row>
-    <row r="85" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A85" s="1">
         <v>2012</v>
       </c>
       <c r="B85" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C85" s="1">
         <f t="shared" si="1"/>
@@ -2554,12 +2554,12 @@
         <v>14926</v>
       </c>
     </row>
-    <row r="86" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A86" s="1">
         <v>2012</v>
       </c>
       <c r="B86" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C86" s="1">
         <f t="shared" si="1"/>
@@ -2578,12 +2578,12 @@
         <v>18994</v>
       </c>
     </row>
-    <row r="87" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A87" s="1">
         <v>2012</v>
       </c>
       <c r="B87" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C87" s="1">
         <f t="shared" si="1"/>
@@ -2602,12 +2602,12 @@
         <v>14520</v>
       </c>
     </row>
-    <row r="88" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A88" s="1">
         <v>2012</v>
       </c>
       <c r="B88" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C88" s="1">
         <f t="shared" si="1"/>
@@ -2626,12 +2626,12 @@
         <v>3912</v>
       </c>
     </row>
-    <row r="89" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A89" s="1">
         <v>2012</v>
       </c>
       <c r="B89" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C89" s="1">
         <f t="shared" si="1"/>
@@ -2650,12 +2650,12 @@
         <v>17354</v>
       </c>
     </row>
-    <row r="90" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A90" s="1">
         <v>2012</v>
       </c>
       <c r="B90" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C90" s="1">
         <f t="shared" si="1"/>
@@ -2674,12 +2674,12 @@
         <v>7590</v>
       </c>
     </row>
-    <row r="91" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A91" s="1">
         <v>2012</v>
       </c>
       <c r="B91" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C91" s="1">
         <f t="shared" si="1"/>
@@ -2698,12 +2698,12 @@
         <v>4942</v>
       </c>
     </row>
-    <row r="92" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A92" s="1">
         <v>2012</v>
       </c>
       <c r="B92" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C92" s="1">
         <f t="shared" si="1"/>
@@ -2722,12 +2722,12 @@
         <v>3025</v>
       </c>
     </row>
-    <row r="93" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A93" s="1">
         <v>2012</v>
       </c>
       <c r="B93" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C93" s="1">
         <f t="shared" si="1"/>
@@ -2746,12 +2746,12 @@
         <v>5682</v>
       </c>
     </row>
-    <row r="94" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A94" s="1">
         <v>2012</v>
       </c>
       <c r="B94" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C94" s="1">
         <f t="shared" si="1"/>
@@ -2770,12 +2770,12 @@
         <v>4546</v>
       </c>
     </row>
-    <row r="95" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A95" s="1">
         <v>2012</v>
       </c>
       <c r="B95" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C95" s="1">
         <f t="shared" si="1"/>
@@ -2794,12 +2794,12 @@
         <v>5848</v>
       </c>
     </row>
-    <row r="96" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A96" s="1">
         <v>2012</v>
       </c>
       <c r="B96" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C96" s="1">
         <f t="shared" si="1"/>
@@ -2818,12 +2818,12 @@
         <v>56</v>
       </c>
     </row>
-    <row r="97" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A97" s="1">
         <v>2012</v>
       </c>
       <c r="B97" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C97" s="1">
         <v>87</v>
@@ -2842,12 +2842,12 @@
         <v>20</v>
       </c>
     </row>
-    <row r="98" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A98" s="1">
         <v>2013</v>
       </c>
       <c r="B98" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C98" s="1">
         <v>65920</v>
@@ -2865,12 +2865,12 @@
         <v>32513</v>
       </c>
     </row>
-    <row r="99" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A99" s="1">
         <v>2013</v>
       </c>
       <c r="B99" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C99" s="1">
         <v>4202</v>
@@ -2888,12 +2888,12 @@
         <v>2049</v>
       </c>
     </row>
-    <row r="100" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A100" s="1">
         <v>2013</v>
       </c>
       <c r="B100" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C100" s="1">
         <v>7004</v>
@@ -2911,12 +2911,12 @@
         <v>3473</v>
       </c>
     </row>
-    <row r="101" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A101" s="1">
         <v>2013</v>
       </c>
       <c r="B101" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C101" s="1">
         <v>15755</v>
@@ -2934,12 +2934,12 @@
         <v>7738</v>
       </c>
     </row>
-    <row r="102" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A102" s="1">
         <v>2013</v>
       </c>
       <c r="B102" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C102" s="1">
         <v>16401</v>
@@ -2957,12 +2957,12 @@
         <v>8044</v>
       </c>
     </row>
-    <row r="103" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A103" s="1">
         <v>2013</v>
       </c>
       <c r="B103" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C103" s="1">
         <v>9478</v>
@@ -2980,12 +2980,12 @@
         <v>4674</v>
       </c>
     </row>
-    <row r="104" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A104" s="1">
         <v>2013</v>
       </c>
       <c r="B104" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C104" s="1">
         <v>10051</v>
@@ -3003,12 +3003,12 @@
         <v>4925</v>
       </c>
     </row>
-    <row r="105" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A105" s="1">
         <v>2013</v>
       </c>
       <c r="B105" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C105" s="1">
         <v>12239</v>
@@ -3026,12 +3026,12 @@
         <v>6088</v>
       </c>
     </row>
-    <row r="106" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A106" s="1">
         <v>2013</v>
       </c>
       <c r="B106" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C106" s="1">
         <v>20265</v>
@@ -3049,12 +3049,12 @@
         <v>9974</v>
       </c>
     </row>
-    <row r="107" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A107" s="1">
         <v>2013</v>
       </c>
       <c r="B107" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C107" s="1">
         <v>13920</v>
@@ -3072,12 +3072,12 @@
         <v>6825</v>
       </c>
     </row>
-    <row r="108" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A108" s="1">
         <v>2013</v>
       </c>
       <c r="B108" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C108" s="1">
         <v>8158</v>
@@ -3095,12 +3095,12 @@
         <v>4060</v>
       </c>
     </row>
-    <row r="109" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A109" s="1">
         <v>2013</v>
       </c>
       <c r="B109" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C109" s="1">
         <v>30193</v>
@@ -3118,12 +3118,12 @@
         <v>14908</v>
       </c>
     </row>
-    <row r="110" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A110" s="1">
         <v>2013</v>
       </c>
       <c r="B110" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C110" s="1">
         <v>37732</v>
@@ -3141,12 +3141,12 @@
         <v>18781</v>
       </c>
     </row>
-    <row r="111" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A111" s="1">
         <v>2013</v>
       </c>
       <c r="B111" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C111" s="1">
         <v>29359</v>
@@ -3164,12 +3164,12 @@
         <v>14329</v>
       </c>
     </row>
-    <row r="112" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A112" s="1">
         <v>2013</v>
       </c>
       <c r="B112" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C112" s="1">
         <v>7889</v>
@@ -3187,12 +3187,12 @@
         <v>3783</v>
       </c>
     </row>
-    <row r="113" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A113" s="1">
         <v>2013</v>
       </c>
       <c r="B113" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C113" s="1">
         <v>34119</v>
@@ -3210,12 +3210,12 @@
         <v>16961</v>
       </c>
     </row>
-    <row r="114" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A114" s="1">
         <v>2013</v>
       </c>
       <c r="B114" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C114" s="1">
         <v>15510</v>
@@ -3233,12 +3233,12 @@
         <v>7641</v>
       </c>
     </row>
-    <row r="115" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="115" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A115" s="1">
         <v>2013</v>
       </c>
       <c r="B115" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C115" s="1">
         <v>10404</v>
@@ -3256,12 +3256,12 @@
         <v>5181</v>
       </c>
     </row>
-    <row r="116" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A116" s="1">
         <v>2013</v>
       </c>
       <c r="B116" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C116" s="1">
         <v>6132</v>
@@ -3279,12 +3279,12 @@
         <v>2997</v>
       </c>
     </row>
-    <row r="117" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A117" s="1">
         <v>2013</v>
       </c>
       <c r="B117" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C117" s="1">
         <v>10954</v>
@@ -3302,12 +3302,12 @@
         <v>5331</v>
       </c>
     </row>
-    <row r="118" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="118" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A118" s="1">
         <v>2013</v>
       </c>
       <c r="B118" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C118" s="1">
         <v>9556</v>
@@ -3325,12 +3325,12 @@
         <v>4700</v>
       </c>
     </row>
-    <row r="119" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="119" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A119" s="1">
         <v>2013</v>
       </c>
       <c r="B119" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C119" s="1">
         <v>11836</v>
@@ -3348,12 +3348,12 @@
         <v>5927</v>
       </c>
     </row>
-    <row r="120" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A120" s="1">
         <v>2013</v>
       </c>
       <c r="B120" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C120" s="1">
         <v>225</v>
@@ -3371,12 +3371,12 @@
         <v>115</v>
       </c>
     </row>
-    <row r="121" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="121" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A121" s="1">
         <v>2013</v>
       </c>
       <c r="B121" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C121" s="1">
         <v>40</v>
@@ -3394,12 +3394,12 @@
         <v>26</v>
       </c>
     </row>
-    <row r="122" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="122" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A122" s="1">
         <v>2014</v>
       </c>
       <c r="B122" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C122" s="1">
         <v>66836</v>
@@ -3417,12 +3417,12 @@
         <v>32795</v>
       </c>
     </row>
-    <row r="123" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="123" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A123" s="1">
         <v>2014</v>
       </c>
       <c r="B123" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C123" s="1">
         <v>4238</v>
@@ -3440,12 +3440,12 @@
         <v>2090</v>
       </c>
     </row>
-    <row r="124" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="124" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A124" s="1">
         <v>2014</v>
       </c>
       <c r="B124" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C124" s="1">
         <v>6965</v>
@@ -3463,12 +3463,12 @@
         <v>3382</v>
       </c>
     </row>
-    <row r="125" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="125" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A125" s="1">
         <v>2014</v>
       </c>
       <c r="B125" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C125" s="1">
         <v>15685</v>
@@ -3486,12 +3486,12 @@
         <v>7727</v>
       </c>
     </row>
-    <row r="126" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="126" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A126" s="1">
         <v>2014</v>
       </c>
       <c r="B126" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C126" s="1">
         <v>16976</v>
@@ -3509,12 +3509,12 @@
         <v>8282</v>
       </c>
     </row>
-    <row r="127" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="127" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A127" s="1">
         <v>2014</v>
       </c>
       <c r="B127" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C127" s="1">
         <v>9168</v>
@@ -3532,12 +3532,12 @@
         <v>4515</v>
       </c>
     </row>
-    <row r="128" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="128" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A128" s="1">
         <v>2014</v>
       </c>
       <c r="B128" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C128" s="1">
         <v>10033</v>
@@ -3555,12 +3555,12 @@
         <v>4926</v>
       </c>
     </row>
-    <row r="129" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="129" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A129" s="1">
         <v>2014</v>
       </c>
       <c r="B129" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C129" s="1">
         <v>12200</v>
@@ -3578,12 +3578,12 @@
         <v>5998</v>
       </c>
     </row>
-    <row r="130" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="130" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A130" s="1">
         <v>2014</v>
       </c>
       <c r="B130" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C130" s="1">
         <v>20518</v>
@@ -3601,12 +3601,12 @@
         <v>10130</v>
       </c>
     </row>
-    <row r="131" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="131" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A131" s="1">
         <v>2014</v>
       </c>
       <c r="B131" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C131" s="1">
         <v>13885</v>
@@ -3624,12 +3624,12 @@
         <v>6761</v>
       </c>
     </row>
-    <row r="132" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="132" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A132" s="1">
         <v>2014</v>
       </c>
       <c r="B132" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C132" s="1">
         <v>8321</v>
@@ -3647,12 +3647,12 @@
         <v>4054</v>
       </c>
     </row>
-    <row r="133" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="133" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A133" s="1">
         <v>2014</v>
       </c>
       <c r="B133" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C133" s="1">
         <v>30366</v>
@@ -3670,12 +3670,12 @@
         <v>14925</v>
       </c>
     </row>
-    <row r="134" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="134" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A134" s="1">
         <v>2014</v>
       </c>
       <c r="B134" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C134" s="1">
         <v>37843</v>
@@ -3693,12 +3693,12 @@
         <v>18589</v>
       </c>
     </row>
-    <row r="135" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="135" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A135" s="1">
         <v>2014</v>
       </c>
       <c r="B135" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C135" s="1">
         <v>28993</v>
@@ -3716,12 +3716,12 @@
         <v>14304</v>
       </c>
     </row>
-    <row r="136" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="136" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A136" s="1">
         <v>2014</v>
       </c>
       <c r="B136" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C136" s="1">
         <v>7941</v>
@@ -3739,12 +3739,12 @@
         <v>3813</v>
       </c>
     </row>
-    <row r="137" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="137" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A137" s="1">
         <v>2014</v>
       </c>
       <c r="B137" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C137" s="1">
         <v>33111</v>
@@ -3762,12 +3762,12 @@
         <v>16252</v>
       </c>
     </row>
-    <row r="138" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="138" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A138" s="1">
         <v>2014</v>
       </c>
       <c r="B138" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C138" s="1">
         <v>15377</v>
@@ -3785,12 +3785,12 @@
         <v>7515</v>
       </c>
     </row>
-    <row r="139" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="139" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A139" s="1">
         <v>2014</v>
       </c>
       <c r="B139" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C139" s="1">
         <v>10140</v>
@@ -3808,12 +3808,12 @@
         <v>5021</v>
       </c>
     </row>
-    <row r="140" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="140" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A140" s="1">
         <v>2014</v>
       </c>
       <c r="B140" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C140" s="1">
         <v>5984</v>
@@ -3831,12 +3831,12 @@
         <v>2833</v>
       </c>
     </row>
-    <row r="141" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="141" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A141" s="1">
         <v>2014</v>
       </c>
       <c r="B141" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C141" s="1">
         <v>10770</v>
@@ -3854,12 +3854,12 @@
         <v>5300</v>
       </c>
     </row>
-    <row r="142" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="142" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A142" s="1">
         <v>2014</v>
       </c>
       <c r="B142" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C142" s="1">
         <v>9448</v>
@@ -3877,12 +3877,12 @@
         <v>4675</v>
       </c>
     </row>
-    <row r="143" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="143" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A143" s="1">
         <v>2014</v>
       </c>
       <c r="B143" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C143" s="1">
         <v>11186</v>
@@ -3900,12 +3900,12 @@
         <v>5527</v>
       </c>
     </row>
-    <row r="144" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="144" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A144" s="1">
         <v>2014</v>
       </c>
       <c r="B144" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C144" s="1">
         <v>155</v>
@@ -3923,12 +3923,12 @@
         <v>70</v>
       </c>
     </row>
-    <row r="145" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="145" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A145" s="1">
         <v>2014</v>
       </c>
       <c r="B145" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C145" s="1">
         <v>56</v>
@@ -3946,12 +3946,12 @@
         <v>26</v>
       </c>
     </row>
-    <row r="146" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="146" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A146" s="1">
         <v>2015</v>
       </c>
       <c r="B146" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C146" s="1">
         <v>67471</v>
@@ -3969,12 +3969,12 @@
         <v>33267</v>
       </c>
     </row>
-    <row r="147" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="147" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A147" s="1">
         <v>2015</v>
       </c>
       <c r="B147" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C147" s="1">
         <v>4057</v>
@@ -3992,12 +3992,12 @@
         <v>1959</v>
       </c>
     </row>
-    <row r="148" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="148" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A148" s="1">
         <v>2015</v>
       </c>
       <c r="B148" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C148" s="1">
         <v>7292</v>
@@ -4015,12 +4015,12 @@
         <v>3629</v>
       </c>
     </row>
-    <row r="149" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="149" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A149" s="1">
         <v>2015</v>
       </c>
       <c r="B149" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C149" s="1">
         <v>16042</v>
@@ -4038,12 +4038,12 @@
         <v>7917</v>
       </c>
     </row>
-    <row r="150" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="150" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A150" s="1">
         <v>2015</v>
       </c>
       <c r="B150" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C150" s="1">
         <v>16830</v>
@@ -4061,12 +4061,12 @@
         <v>8297</v>
       </c>
     </row>
-    <row r="151" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="151" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A151" s="1">
         <v>2015</v>
       </c>
       <c r="B151" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C151" s="1">
         <v>8834</v>
@@ -4084,12 +4084,12 @@
         <v>4434</v>
       </c>
     </row>
-    <row r="152" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="152" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A152" s="1">
         <v>2015</v>
       </c>
       <c r="B152" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C152" s="1">
         <v>10507</v>
@@ -4107,12 +4107,12 @@
         <v>5124</v>
       </c>
     </row>
-    <row r="153" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="153" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A153" s="1">
         <v>2015</v>
       </c>
       <c r="B153" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C153" s="1">
         <v>12443</v>
@@ -4130,12 +4130,12 @@
         <v>6053</v>
       </c>
     </row>
-    <row r="154" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="154" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A154" s="1">
         <v>2015</v>
       </c>
       <c r="B154" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C154" s="1">
         <v>20838</v>
@@ -4153,12 +4153,12 @@
         <v>10341</v>
       </c>
     </row>
-    <row r="155" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="155" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A155" s="1">
         <v>2015</v>
       </c>
       <c r="B155" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C155" s="1">
         <v>13818</v>
@@ -4176,12 +4176,12 @@
         <v>6686</v>
       </c>
     </row>
-    <row r="156" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="156" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A156" s="1">
         <v>2015</v>
       </c>
       <c r="B156" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C156" s="1">
         <v>8510</v>
@@ -4199,12 +4199,12 @@
         <v>4150</v>
       </c>
     </row>
-    <row r="157" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="157" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A157" s="1">
         <v>2015</v>
       </c>
       <c r="B157" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C157" s="1">
         <v>30832</v>
@@ -4222,12 +4222,12 @@
         <v>15087</v>
       </c>
     </row>
-    <row r="158" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="158" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A158" s="1">
         <v>2015</v>
       </c>
       <c r="B158" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C158" s="1">
         <v>38669</v>
@@ -4245,12 +4245,12 @@
         <v>19056</v>
       </c>
     </row>
-    <row r="159" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="159" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A159" s="1">
         <v>2015</v>
       </c>
       <c r="B159" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C159" s="1">
         <v>29490</v>
@@ -4268,12 +4268,12 @@
         <v>14523</v>
       </c>
     </row>
-    <row r="160" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="160" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A160" s="1">
         <v>2015</v>
       </c>
       <c r="B160" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C160" s="1">
         <v>7953</v>
@@ -4291,12 +4291,12 @@
         <v>3825</v>
       </c>
     </row>
-    <row r="161" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="161" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A161" s="1">
         <v>2015</v>
       </c>
       <c r="B161" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C161" s="1">
         <v>34605</v>
@@ -4314,12 +4314,12 @@
         <v>17092</v>
       </c>
     </row>
-    <row r="162" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="162" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A162" s="1">
         <v>2015</v>
       </c>
       <c r="B162" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C162" s="1">
         <v>15111</v>
@@ -4337,12 +4337,12 @@
         <v>7523</v>
       </c>
     </row>
-    <row r="163" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="163" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A163" s="1">
         <v>2015</v>
       </c>
       <c r="B163" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C163" s="1">
         <v>10326</v>
@@ -4360,12 +4360,12 @@
         <v>5121</v>
       </c>
     </row>
-    <row r="164" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="164" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A164" s="1">
         <v>2015</v>
       </c>
       <c r="B164" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C164" s="1">
         <v>6115</v>
@@ -4383,12 +4383,12 @@
         <v>3040</v>
       </c>
     </row>
-    <row r="165" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="165" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A165" s="1">
         <v>2015</v>
       </c>
       <c r="B165" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C165" s="1">
         <v>10967</v>
@@ -4406,12 +4406,12 @@
         <v>5447</v>
       </c>
     </row>
-    <row r="166" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="166" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A166" s="1">
         <v>2015</v>
       </c>
       <c r="B166" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C166" s="1">
         <v>9340</v>
@@ -4429,12 +4429,12 @@
         <v>4561</v>
       </c>
     </row>
-    <row r="167" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="167" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A167" s="1">
         <v>2015</v>
       </c>
       <c r="B167" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C167" s="1">
         <v>11239</v>
@@ -4452,12 +4452,12 @@
         <v>5480</v>
       </c>
     </row>
-    <row r="168" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="168" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A168" s="1">
         <v>2015</v>
       </c>
       <c r="B168" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C168" s="1">
         <v>107</v>
@@ -4475,12 +4475,12 @@
         <v>44</v>
       </c>
     </row>
-    <row r="169" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="169" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A169" s="1">
         <v>2015</v>
       </c>
       <c r="B169" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C169" s="1">
         <v>29</v>
@@ -4498,12 +4498,12 @@
         <v>19</v>
       </c>
     </row>
-    <row r="170" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="170" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A170" s="1">
         <v>2016</v>
       </c>
       <c r="B170" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C170" s="1">
         <v>67192</v>
@@ -4521,12 +4521,12 @@
         <v>32830</v>
       </c>
     </row>
-    <row r="171" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="171" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A171" s="1">
         <v>2016</v>
       </c>
       <c r="B171" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C171" s="1">
         <v>4044</v>
@@ -4544,12 +4544,12 @@
         <v>1954</v>
       </c>
     </row>
-    <row r="172" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="172" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A172" s="1">
         <v>2016</v>
       </c>
       <c r="B172" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C172" s="1">
         <v>6734</v>
@@ -4567,12 +4567,12 @@
         <v>3237</v>
       </c>
     </row>
-    <row r="173" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="173" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A173" s="1">
         <v>2016</v>
       </c>
       <c r="B173" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C173" s="1">
         <v>16563</v>
@@ -4590,12 +4590,12 @@
         <v>8125</v>
       </c>
     </row>
-    <row r="174" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="174" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A174" s="1">
         <v>2016</v>
       </c>
       <c r="B174" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C174" s="1">
         <v>16266</v>
@@ -4613,12 +4613,12 @@
         <v>8062</v>
       </c>
     </row>
-    <row r="175" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="175" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A175" s="1">
         <v>2016</v>
       </c>
       <c r="B175" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C175" s="1">
         <v>9063</v>
@@ -4636,12 +4636,12 @@
         <v>4501</v>
       </c>
     </row>
-    <row r="176" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="176" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A176" s="1">
         <v>2016</v>
       </c>
       <c r="B176" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C176" s="1">
         <v>10351</v>
@@ -4659,12 +4659,12 @@
         <v>5110</v>
       </c>
     </row>
-    <row r="177" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="177" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A177" s="1">
         <v>2016</v>
       </c>
       <c r="B177" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C177" s="1">
         <v>13113</v>
@@ -4682,12 +4682,12 @@
         <v>6396</v>
       </c>
     </row>
-    <row r="178" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="178" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A178" s="1">
         <v>2016</v>
       </c>
       <c r="B178" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C178" s="1">
         <v>20774</v>
@@ -4705,12 +4705,12 @@
         <v>10154</v>
       </c>
     </row>
-    <row r="179" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="179" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A179" s="1">
         <v>2016</v>
       </c>
       <c r="B179" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C179" s="1">
         <v>13349</v>
@@ -4728,12 +4728,12 @@
         <v>6535</v>
       </c>
     </row>
-    <row r="180" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="180" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A180" s="1">
         <v>2016</v>
       </c>
       <c r="B180" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C180" s="1">
         <v>8144</v>
@@ -4751,12 +4751,12 @@
         <v>4024</v>
       </c>
     </row>
-    <row r="181" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="181" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A181" s="1">
         <v>2016</v>
       </c>
       <c r="B181" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C181" s="1">
         <v>31880</v>
@@ -4774,12 +4774,12 @@
         <v>15638</v>
       </c>
     </row>
-    <row r="182" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="182" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A182" s="1">
         <v>2016</v>
       </c>
       <c r="B182" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C182" s="1">
         <v>38078</v>
@@ -4797,12 +4797,12 @@
         <v>18691</v>
       </c>
     </row>
-    <row r="183" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="183" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A183" s="1">
         <v>2016</v>
       </c>
       <c r="B183" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C183" s="1">
         <v>29490</v>
@@ -4820,12 +4820,12 @@
         <v>14615</v>
       </c>
     </row>
-    <row r="184" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="184" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A184" s="1">
         <v>2016</v>
       </c>
       <c r="B184" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C184" s="1">
         <v>8187</v>
@@ -4843,12 +4843,12 @@
         <v>3972</v>
       </c>
     </row>
-    <row r="185" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="185" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A185" s="1">
         <v>2016</v>
       </c>
       <c r="B185" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C185" s="1">
         <v>34340</v>
@@ -4866,12 +4866,12 @@
         <v>17060</v>
       </c>
     </row>
-    <row r="186" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="186" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A186" s="1">
         <v>2016</v>
       </c>
       <c r="B186" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C186" s="1">
         <v>15474</v>
@@ -4889,12 +4889,12 @@
         <v>7597</v>
       </c>
     </row>
-    <row r="187" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="187" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A187" s="1">
         <v>2016</v>
       </c>
       <c r="B187" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C187" s="1">
         <v>9800</v>
@@ -4912,12 +4912,12 @@
         <v>4825</v>
       </c>
     </row>
-    <row r="188" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="188" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A188" s="1">
         <v>2016</v>
       </c>
       <c r="B188" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C188" s="1">
         <v>5443</v>
@@ -4935,12 +4935,12 @@
         <v>2646</v>
       </c>
     </row>
-    <row r="189" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="189" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A189" s="1">
         <v>2016</v>
       </c>
       <c r="B189" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C189" s="1">
         <v>11375</v>
@@ -4958,12 +4958,12 @@
         <v>5637</v>
       </c>
     </row>
-    <row r="190" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="190" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A190" s="1">
         <v>2016</v>
       </c>
       <c r="B190" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C190" s="1">
         <v>9303</v>
@@ -4981,12 +4981,12 @@
         <v>4553</v>
       </c>
     </row>
-    <row r="191" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="191" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A191" s="1">
         <v>2016</v>
       </c>
       <c r="B191" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C191" s="1">
         <v>11246</v>
@@ -5004,12 +5004,12 @@
         <v>5619</v>
       </c>
     </row>
-    <row r="192" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="192" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A192" s="1">
         <v>2016</v>
       </c>
       <c r="B192" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C192" s="1">
         <v>130</v>
@@ -5027,12 +5027,12 @@
         <v>61</v>
       </c>
     </row>
-    <row r="193" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="193" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A193" s="1">
         <v>2016</v>
       </c>
       <c r="B193" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C193" s="1">
         <v>43</v>
@@ -5050,12 +5050,12 @@
         <v>24</v>
       </c>
     </row>
-    <row r="194" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="194" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A194" s="1">
         <v>2017</v>
       </c>
       <c r="B194" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C194" s="1">
         <v>66407</v>
@@ -5073,12 +5073,12 @@
         <v>32476</v>
       </c>
     </row>
-    <row r="195" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="195" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A195" s="1">
         <v>2017</v>
       </c>
       <c r="B195" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C195" s="1">
         <v>3990</v>
@@ -5096,12 +5096,12 @@
         <v>1978</v>
       </c>
     </row>
-    <row r="196" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="196" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A196" s="1">
         <v>2017</v>
       </c>
       <c r="B196" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C196" s="1">
         <v>6631</v>
@@ -5119,12 +5119,12 @@
         <v>3249</v>
       </c>
     </row>
-    <row r="197" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="197" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A197" s="1">
         <v>2017</v>
       </c>
       <c r="B197" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C197" s="1">
         <v>15824</v>
@@ -5142,12 +5142,12 @@
         <v>7766</v>
       </c>
     </row>
-    <row r="198" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="198" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A198" s="1">
         <v>2017</v>
       </c>
       <c r="B198" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C198" s="1">
         <v>16249</v>
@@ -5165,12 +5165,12 @@
         <v>7957</v>
       </c>
     </row>
-    <row r="199" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="199" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A199" s="1">
         <v>2017</v>
       </c>
       <c r="B199" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C199" s="1">
         <v>8464</v>
@@ -5188,12 +5188,12 @@
         <v>4129</v>
       </c>
     </row>
-    <row r="200" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="200" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A200" s="1">
         <v>2017</v>
       </c>
       <c r="B200" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C200" s="1">
         <v>10209</v>
@@ -5211,12 +5211,12 @@
         <v>5074</v>
       </c>
     </row>
-    <row r="201" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="201" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A201" s="1">
         <v>2017</v>
       </c>
       <c r="B201" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C201" s="1">
         <v>12744</v>
@@ -5234,12 +5234,12 @@
         <v>6155</v>
       </c>
     </row>
-    <row r="202" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="202" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A202" s="1">
         <v>2017</v>
       </c>
       <c r="B202" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C202" s="1">
         <v>20248</v>
@@ -5257,12 +5257,12 @@
         <v>9951</v>
       </c>
     </row>
-    <row r="203" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="203" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A203" s="1">
         <v>2017</v>
       </c>
       <c r="B203" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C203" s="1">
         <v>13549</v>
@@ -5280,12 +5280,12 @@
         <v>6671</v>
       </c>
     </row>
-    <row r="204" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="204" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A204" s="1">
         <v>2017</v>
       </c>
       <c r="B204" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C204" s="1">
         <v>8115</v>
@@ -5303,12 +5303,12 @@
         <v>4011</v>
       </c>
     </row>
-    <row r="205" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="205" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A205" s="1">
         <v>2017</v>
       </c>
       <c r="B205" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C205" s="1">
         <v>30133</v>
@@ -5326,12 +5326,12 @@
         <v>14796</v>
       </c>
     </row>
-    <row r="206" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="206" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A206" s="1">
         <v>2017</v>
       </c>
       <c r="B206" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C206" s="1">
         <v>37607</v>
@@ -5349,12 +5349,12 @@
         <v>18543</v>
       </c>
     </row>
-    <row r="207" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="207" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A207" s="1">
         <v>2017</v>
       </c>
       <c r="B207" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C207" s="1">
         <v>28651</v>
@@ -5372,12 +5372,12 @@
         <v>14041</v>
       </c>
     </row>
-    <row r="208" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="208" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A208" s="1">
         <v>2017</v>
       </c>
       <c r="B208" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C208" s="1">
         <v>7912</v>
@@ -5395,12 +5395,12 @@
         <v>3932</v>
       </c>
     </row>
-    <row r="209" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="209" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A209" s="1">
         <v>2017</v>
       </c>
       <c r="B209" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C209" s="1">
         <v>33966</v>
@@ -5418,12 +5418,12 @@
         <v>16519</v>
       </c>
     </row>
-    <row r="210" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="210" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A210" s="1">
         <v>2017</v>
       </c>
       <c r="B210" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C210" s="1">
         <v>14808</v>
@@ -5441,12 +5441,12 @@
         <v>7272</v>
       </c>
     </row>
-    <row r="211" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="211" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A211" s="1">
         <v>2017</v>
       </c>
       <c r="B211" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C211" s="1">
         <v>9789</v>
@@ -5464,12 +5464,12 @@
         <v>4855</v>
       </c>
     </row>
-    <row r="212" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="212" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A212" s="1">
         <v>2017</v>
       </c>
       <c r="B212" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C212" s="1">
         <v>5885</v>
@@ -5487,12 +5487,12 @@
         <v>2858</v>
       </c>
     </row>
-    <row r="213" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="213" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A213" s="1">
         <v>2017</v>
       </c>
       <c r="B213" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C213" s="1">
         <v>10495</v>
@@ -5510,12 +5510,12 @@
         <v>5174</v>
       </c>
     </row>
-    <row r="214" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="214" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A214" s="1">
         <v>2017</v>
       </c>
       <c r="B214" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C214" s="1">
         <v>8972</v>
@@ -5533,12 +5533,12 @@
         <v>4370</v>
       </c>
     </row>
-    <row r="215" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="215" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A215" s="1">
         <v>2017</v>
       </c>
       <c r="B215" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C215" s="1">
         <v>10748</v>
@@ -5556,12 +5556,12 @@
         <v>5243</v>
       </c>
     </row>
-    <row r="216" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="216" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A216" s="1">
         <v>2017</v>
       </c>
       <c r="B216" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C216" s="1">
         <v>194</v>
@@ -5579,12 +5579,12 @@
         <v>97</v>
       </c>
     </row>
-    <row r="217" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="217" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A217" s="1">
         <v>2017</v>
       </c>
       <c r="B217" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C217" s="1">
         <v>74</v>
@@ -5602,12 +5602,12 @@
         <v>41</v>
       </c>
     </row>
-    <row r="218" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="218" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A218" s="1">
         <v>2018</v>
       </c>
       <c r="B218" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C218" s="1">
         <v>64735</v>
@@ -5625,12 +5625,12 @@
         <v>32045</v>
       </c>
     </row>
-    <row r="219" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="219" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A219" s="1">
         <v>2018</v>
       </c>
       <c r="B219" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C219" s="1">
         <v>3920</v>
@@ -5648,12 +5648,12 @@
         <v>1853</v>
       </c>
     </row>
-    <row r="220" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="220" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A220" s="1">
         <v>2018</v>
       </c>
       <c r="B220" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C220" s="1">
         <v>6545</v>
@@ -5671,12 +5671,12 @@
         <v>3200</v>
       </c>
     </row>
-    <row r="221" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="221" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A221" s="1">
         <v>2018</v>
       </c>
       <c r="B221" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C221" s="1">
         <v>15540</v>
@@ -5694,12 +5694,12 @@
         <v>7648</v>
       </c>
     </row>
-    <row r="222" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="222" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A222" s="1">
         <v>2018</v>
       </c>
       <c r="B222" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C222" s="1">
         <v>16321</v>
@@ -5717,12 +5717,12 @@
         <v>7904</v>
       </c>
     </row>
-    <row r="223" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="223" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A223" s="1">
         <v>2018</v>
       </c>
       <c r="B223" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C223" s="1">
         <v>8228</v>
@@ -5740,12 +5740,12 @@
         <v>4017</v>
       </c>
     </row>
-    <row r="224" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="224" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A224" s="1">
         <v>2018</v>
       </c>
       <c r="B224" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C224" s="1">
         <v>10168</v>
@@ -5763,12 +5763,12 @@
         <v>4985</v>
       </c>
     </row>
-    <row r="225" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="225" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A225" s="1">
         <v>2018</v>
       </c>
       <c r="B225" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C225" s="1">
         <v>12945</v>
@@ -5786,12 +5786,12 @@
         <v>6335</v>
       </c>
     </row>
-    <row r="226" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="226" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A226" s="1">
         <v>2018</v>
       </c>
       <c r="B226" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C226" s="1">
         <v>20050</v>
@@ -5809,12 +5809,12 @@
         <v>9859</v>
       </c>
     </row>
-    <row r="227" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="227" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A227" s="1">
         <v>2018</v>
       </c>
       <c r="B227" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C227" s="1">
         <v>13623</v>
@@ -5832,12 +5832,12 @@
         <v>6624</v>
       </c>
     </row>
-    <row r="228" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="228" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A228" s="1">
         <v>2018</v>
       </c>
       <c r="B228" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C228" s="1">
         <v>8236</v>
@@ -5855,12 +5855,12 @@
         <v>4027</v>
       </c>
     </row>
-    <row r="229" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="229" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A229" s="1">
         <v>2018</v>
       </c>
       <c r="B229" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C229" s="1">
         <v>29426</v>
@@ -5878,12 +5878,12 @@
         <v>14468</v>
       </c>
     </row>
-    <row r="230" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="230" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A230" s="1">
         <v>2018</v>
       </c>
       <c r="B230" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C230" s="1">
         <v>38156</v>
@@ -5901,12 +5901,12 @@
         <v>18777</v>
       </c>
     </row>
-    <row r="231" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="231" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A231" s="1">
         <v>2018</v>
       </c>
       <c r="B231" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C231" s="1">
         <v>30168</v>
@@ -5924,12 +5924,12 @@
         <v>14808</v>
       </c>
     </row>
-    <row r="232" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="232" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A232" s="1">
         <v>2018</v>
       </c>
       <c r="B232" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C232" s="1">
         <v>8030</v>
@@ -5947,12 +5947,12 @@
         <v>3945</v>
       </c>
     </row>
-    <row r="233" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="233" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A233" s="1">
         <v>2018</v>
       </c>
       <c r="B233" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C233" s="1">
         <v>34819</v>
@@ -5970,12 +5970,12 @@
         <v>17162</v>
       </c>
     </row>
-    <row r="234" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="234" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A234" s="1">
         <v>2018</v>
       </c>
       <c r="B234" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C234" s="1">
         <v>15427</v>
@@ -5993,12 +5993,12 @@
         <v>7597</v>
       </c>
     </row>
-    <row r="235" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="235" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A235" s="1">
         <v>2018</v>
       </c>
       <c r="B235" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C235" s="1">
         <v>10130</v>
@@ -6016,12 +6016,12 @@
         <v>5029</v>
       </c>
     </row>
-    <row r="236" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="236" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A236" s="1">
         <v>2018</v>
       </c>
       <c r="B236" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C236" s="1">
         <v>5835</v>
@@ -6039,12 +6039,12 @@
         <v>2918</v>
       </c>
     </row>
-    <row r="237" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="237" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A237" s="1">
         <v>2018</v>
       </c>
       <c r="B237" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C237" s="1">
         <v>10698</v>
@@ -6062,12 +6062,12 @@
         <v>5234</v>
       </c>
     </row>
-    <row r="238" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="238" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A238" s="1">
         <v>2018</v>
       </c>
       <c r="B238" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C238" s="1">
         <v>9305</v>
@@ -6085,12 +6085,12 @@
         <v>4542</v>
       </c>
     </row>
-    <row r="239" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="239" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A239" s="1">
         <v>2018</v>
       </c>
       <c r="B239" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C239" s="1">
         <v>10536</v>
@@ -6108,12 +6108,12 @@
         <v>5163</v>
       </c>
     </row>
-    <row r="240" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="240" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A240" s="1">
         <v>2018</v>
       </c>
       <c r="B240" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C240" s="1">
         <v>339</v>
@@ -6131,12 +6131,12 @@
         <v>159</v>
       </c>
     </row>
-    <row r="241" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="241" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A241" s="1">
         <v>2018</v>
       </c>
       <c r="B241" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C241" s="1">
         <v>83</v>
@@ -6154,12 +6154,12 @@
         <v>41</v>
       </c>
     </row>
-    <row r="242" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="242" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A242" s="1">
         <v>2019</v>
       </c>
       <c r="B242" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C242" s="1">
         <v>59563</v>
@@ -6177,12 +6177,12 @@
         <v>29422</v>
       </c>
     </row>
-    <row r="243" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="243" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A243" s="1">
         <v>2019</v>
       </c>
       <c r="B243" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C243" s="1">
         <v>3709</v>
@@ -6200,12 +6200,12 @@
         <v>1829</v>
       </c>
     </row>
-    <row r="244" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="244" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A244" s="1">
         <v>2019</v>
       </c>
       <c r="B244" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C244" s="1">
         <v>6341</v>
@@ -6223,12 +6223,12 @@
         <v>3111</v>
       </c>
     </row>
-    <row r="245" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="245" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A245" s="1">
         <v>2019</v>
       </c>
       <c r="B245" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C245" s="1">
         <v>15192</v>
@@ -6246,12 +6246,12 @@
         <v>7385</v>
       </c>
     </row>
-    <row r="246" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="246" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A246" s="1">
         <v>2019</v>
       </c>
       <c r="B246" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C246" s="1">
         <v>15437</v>
@@ -6269,12 +6269,12 @@
         <v>7493</v>
       </c>
     </row>
-    <row r="247" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="247" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A247" s="1">
         <v>2019</v>
       </c>
       <c r="B247" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C247" s="1">
         <v>8024</v>
@@ -6292,12 +6292,12 @@
         <v>3998</v>
       </c>
     </row>
-    <row r="248" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="248" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A248" s="1">
         <v>2019</v>
       </c>
       <c r="B248" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C248" s="1">
         <v>10021</v>
@@ -6315,12 +6315,12 @@
         <v>4896</v>
       </c>
     </row>
-    <row r="249" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="249" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A249" s="1">
         <v>2019</v>
       </c>
       <c r="B249" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C249" s="1">
         <v>12507</v>
@@ -6338,12 +6338,12 @@
         <v>6089</v>
       </c>
     </row>
-    <row r="250" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="250" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A250" s="1">
         <v>2019</v>
       </c>
       <c r="B250" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C250" s="1">
         <v>19461</v>
@@ -6361,12 +6361,12 @@
         <v>9658</v>
       </c>
     </row>
-    <row r="251" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="251" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A251" s="1">
         <v>2019</v>
       </c>
       <c r="B251" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C251" s="1">
         <v>13252</v>
@@ -6384,12 +6384,12 @@
         <v>6511</v>
       </c>
     </row>
-    <row r="252" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="252" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A252" s="1">
         <v>2019</v>
       </c>
       <c r="B252" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C252" s="1">
         <v>7752</v>
@@ -6407,12 +6407,12 @@
         <v>3756</v>
       </c>
     </row>
-    <row r="253" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="253" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A253" s="1">
         <v>2019</v>
       </c>
       <c r="B253" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C253" s="1">
         <v>27460</v>
@@ -6430,12 +6430,12 @@
         <v>13491</v>
       </c>
     </row>
-    <row r="254" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="254" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A254" s="1">
         <v>2019</v>
       </c>
       <c r="B254" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C254" s="1">
         <v>36881</v>
@@ -6453,12 +6453,12 @@
         <v>18131</v>
       </c>
     </row>
-    <row r="255" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="255" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A255" s="1">
         <v>2019</v>
       </c>
       <c r="B255" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C255" s="1">
         <v>29288</v>
@@ -6476,12 +6476,12 @@
         <v>14356</v>
       </c>
     </row>
-    <row r="256" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="256" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A256" s="1">
         <v>2019</v>
       </c>
       <c r="B256" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C256" s="1">
         <v>7831</v>
@@ -6499,12 +6499,12 @@
         <v>3843</v>
       </c>
     </row>
-    <row r="257" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="257" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A257" s="1">
         <v>2019</v>
       </c>
       <c r="B257" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C257" s="1">
         <v>34614</v>
@@ -6522,12 +6522,12 @@
         <v>16966</v>
       </c>
     </row>
-    <row r="258" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="258" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A258" s="1">
         <v>2019</v>
       </c>
       <c r="B258" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C258" s="1">
         <v>14851</v>
@@ -6545,12 +6545,12 @@
         <v>7285</v>
       </c>
     </row>
-    <row r="259" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="259" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A259" s="1">
         <v>2019</v>
       </c>
       <c r="B259" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C259" s="1">
         <v>9393</v>
@@ -6568,12 +6568,12 @@
         <v>4664</v>
       </c>
     </row>
-    <row r="260" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="260" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A260" s="1">
         <v>2019</v>
       </c>
       <c r="B260" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C260" s="1">
         <v>5460</v>
@@ -6591,12 +6591,12 @@
         <v>2674</v>
       </c>
     </row>
-    <row r="261" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="261" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A261" s="1">
         <v>2019</v>
       </c>
       <c r="B261" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C261" s="1">
         <v>10123</v>
@@ -6614,12 +6614,12 @@
         <v>5008</v>
       </c>
     </row>
-    <row r="262" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="262" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A262" s="1">
         <v>2019</v>
       </c>
       <c r="B262" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C262" s="1">
         <v>8931</v>
@@ -6637,12 +6637,12 @@
         <v>4367</v>
       </c>
     </row>
-    <row r="263" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="263" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A263" s="1">
         <v>2019</v>
       </c>
       <c r="B263" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C263" s="1">
         <v>10357</v>
@@ -6660,18 +6660,18 @@
         <v>5075</v>
       </c>
     </row>
-    <row r="264" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="264" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A264" s="1">
         <v>2019</v>
       </c>
       <c r="B264" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C264" s="1">
         <v>339</v>
       </c>
       <c r="D264" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E264" s="1">
         <v>339</v>
@@ -6683,12 +6683,12 @@
         <v>169</v>
       </c>
     </row>
-    <row r="265" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="265" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A265" s="1">
         <v>2019</v>
       </c>
       <c r="B265" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C265" s="1">
         <v>68</v>
@@ -6706,12 +6706,12 @@
         <v>37</v>
       </c>
     </row>
-    <row r="266" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="266" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A266" s="1">
         <v>2020</v>
       </c>
       <c r="B266" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C266" s="1">
         <v>54807</v>
@@ -6729,12 +6729,12 @@
         <v>26879</v>
       </c>
     </row>
-    <row r="267" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="267" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A267" s="1">
         <v>2020</v>
       </c>
       <c r="B267" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C267" s="1">
         <v>3560</v>
@@ -6752,12 +6752,12 @@
         <v>1706</v>
       </c>
     </row>
-    <row r="268" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="268" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A268" s="1">
         <v>2020</v>
       </c>
       <c r="B268" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C268" s="1">
         <v>6064</v>
@@ -6775,12 +6775,12 @@
         <v>2981</v>
       </c>
     </row>
-    <row r="269" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="269" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A269" s="1">
         <v>2020</v>
       </c>
       <c r="B269" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C269" s="1">
         <v>14090</v>
@@ -6798,12 +6798,12 @@
         <v>6989</v>
       </c>
     </row>
-    <row r="270" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="270" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A270" s="1">
         <v>2020</v>
       </c>
       <c r="B270" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C270" s="1">
         <v>14102</v>
@@ -6821,12 +6821,12 @@
         <v>6896</v>
       </c>
     </row>
-    <row r="271" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="271" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A271" s="1">
         <v>2020</v>
       </c>
       <c r="B271" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C271" s="1">
         <v>7696</v>
@@ -6844,12 +6844,12 @@
         <v>3749</v>
       </c>
     </row>
-    <row r="272" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="272" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A272" s="1">
         <v>2020</v>
       </c>
       <c r="B272" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C272" s="1">
         <v>9373</v>
@@ -6867,12 +6867,12 @@
         <v>4617</v>
       </c>
     </row>
-    <row r="273" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="273" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A273" s="1">
         <v>2020</v>
       </c>
       <c r="B273" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C273" s="1">
         <v>11838</v>
@@ -6890,12 +6890,12 @@
         <v>5850</v>
       </c>
     </row>
-    <row r="274" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="274" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A274" s="1">
         <v>2020</v>
       </c>
       <c r="B274" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C274" s="1">
         <v>17911</v>
@@ -6913,12 +6913,12 @@
         <v>8976</v>
       </c>
     </row>
-    <row r="275" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="275" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A275" s="1">
         <v>2020</v>
       </c>
       <c r="B275" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C275" s="1">
         <v>12066</v>
@@ -6936,12 +6936,12 @@
         <v>5974</v>
       </c>
     </row>
-    <row r="276" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="276" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A276" s="1">
         <v>2020</v>
       </c>
       <c r="B276" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C276" s="1">
         <v>7075</v>
@@ -6959,12 +6959,12 @@
         <v>3492</v>
       </c>
     </row>
-    <row r="277" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="277" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A277" s="1">
         <v>2020</v>
       </c>
       <c r="B277" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C277" s="1">
         <v>26191</v>
@@ -6982,12 +6982,12 @@
         <v>12756</v>
       </c>
     </row>
-    <row r="278" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="278" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A278" s="1">
         <v>2020</v>
       </c>
       <c r="B278" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C278" s="1">
         <v>33839</v>
@@ -7005,12 +7005,12 @@
         <v>16717</v>
       </c>
     </row>
-    <row r="279" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="279" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A279" s="1">
         <v>2020</v>
       </c>
       <c r="B279" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C279" s="1">
         <v>28045</v>
@@ -7028,12 +7028,12 @@
         <v>13916</v>
       </c>
     </row>
-    <row r="280" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="280" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A280" s="1">
         <v>2020</v>
       </c>
       <c r="B280" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C280" s="1">
         <v>7274</v>
@@ -7051,12 +7051,12 @@
         <v>3590</v>
       </c>
     </row>
-    <row r="281" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="281" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A281" s="1">
         <v>2020</v>
       </c>
       <c r="B281" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C281" s="1">
         <v>31582</v>
@@ -7074,12 +7074,12 @@
         <v>15561</v>
       </c>
     </row>
-    <row r="282" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="282" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A282" s="1">
         <v>2020</v>
       </c>
       <c r="B282" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C282" s="1">
         <v>13358</v>
@@ -7097,12 +7097,12 @@
         <v>6475</v>
       </c>
     </row>
-    <row r="283" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="283" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A283" s="1">
         <v>2020</v>
       </c>
       <c r="B283" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C283" s="1">
         <v>8919</v>
@@ -7120,12 +7120,12 @@
         <v>4441</v>
       </c>
     </row>
-    <row r="284" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="284" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A284" s="1">
         <v>2020</v>
       </c>
       <c r="B284" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C284" s="1">
         <v>5000</v>
@@ -7143,12 +7143,12 @@
         <v>2452</v>
       </c>
     </row>
-    <row r="285" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="285" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A285" s="1">
         <v>2020</v>
       </c>
       <c r="B285" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C285" s="1">
         <v>9693</v>
@@ -7166,12 +7166,12 @@
         <v>4662</v>
       </c>
     </row>
-    <row r="286" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="286" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A286" s="1">
         <v>2020</v>
       </c>
       <c r="B286" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C286" s="1">
         <v>8457</v>
@@ -7189,12 +7189,12 @@
         <v>4130</v>
       </c>
     </row>
-    <row r="287" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="287" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A287" s="1">
         <v>2020</v>
       </c>
       <c r="B287" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C287" s="1">
         <v>9936</v>
@@ -7212,12 +7212,12 @@
         <v>4810</v>
       </c>
     </row>
-    <row r="288" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="288" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A288" s="1">
         <v>2020</v>
       </c>
       <c r="B288" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C288" s="1">
         <v>223</v>
@@ -7235,12 +7235,12 @@
         <v>110</v>
       </c>
     </row>
-    <row r="289" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="289" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A289" s="1">
         <v>2020</v>
       </c>
       <c r="B289" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C289" s="1">
         <v>113</v>
@@ -7258,12 +7258,12 @@
         <v>49</v>
       </c>
     </row>
-    <row r="290" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="290" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A290" s="1">
         <v>2021</v>
       </c>
       <c r="B290" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C290" s="1">
         <v>51191</v>
@@ -7281,12 +7281,12 @@
         <v>25335</v>
       </c>
     </row>
-    <row r="291" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="291" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A291" s="1">
         <v>2021</v>
       </c>
       <c r="B291" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C291" s="1">
         <v>3405</v>
@@ -7304,12 +7304,12 @@
         <v>1702</v>
       </c>
     </row>
-    <row r="292" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="292" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A292" s="1">
         <v>2021</v>
       </c>
       <c r="B292" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C292" s="1">
         <v>5813</v>
@@ -7327,12 +7327,12 @@
         <v>2831</v>
       </c>
     </row>
-    <row r="293" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="293" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A293" s="1">
         <v>2021</v>
       </c>
       <c r="B293" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C293" s="1">
         <v>14151</v>
@@ -7350,12 +7350,12 @@
         <v>7017</v>
       </c>
     </row>
-    <row r="294" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="294" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A294" s="1">
         <v>2021</v>
       </c>
       <c r="B294" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C294" s="1">
         <v>14189</v>
@@ -7373,12 +7373,12 @@
         <v>7074</v>
       </c>
     </row>
-    <row r="295" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="295" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A295" s="1">
         <v>2021</v>
       </c>
       <c r="B295" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C295" s="1">
         <v>7509</v>
@@ -7396,12 +7396,12 @@
         <v>3713</v>
       </c>
     </row>
-    <row r="296" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="296" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A296" s="1">
         <v>2021</v>
       </c>
       <c r="B296" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C296" s="1">
         <v>9602</v>
@@ -7419,12 +7419,12 @@
         <v>4691</v>
       </c>
     </row>
-    <row r="297" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="297" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A297" s="1">
         <v>2021</v>
       </c>
       <c r="B297" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C297" s="1">
         <v>12128</v>
@@ -7442,12 +7442,12 @@
         <v>5900</v>
       </c>
     </row>
-    <row r="298" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="298" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A298" s="1">
         <v>2021</v>
       </c>
       <c r="B298" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C298" s="1">
         <v>17875</v>
@@ -7465,12 +7465,12 @@
         <v>8833</v>
       </c>
     </row>
-    <row r="299" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="299" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A299" s="1">
         <v>2021</v>
       </c>
       <c r="B299" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C299" s="1">
         <v>12264</v>
@@ -7488,12 +7488,12 @@
         <v>6044</v>
       </c>
     </row>
-    <row r="300" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="300" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A300" s="1">
         <v>2021</v>
       </c>
       <c r="B300" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C300" s="1">
         <v>6908</v>
@@ -7511,12 +7511,12 @@
         <v>3394</v>
       </c>
     </row>
-    <row r="301" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="301" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A301" s="1">
         <v>2021</v>
       </c>
       <c r="B301" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C301" s="1">
         <v>26241</v>
@@ -7534,12 +7534,12 @@
         <v>12911</v>
       </c>
     </row>
-    <row r="302" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="302" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A302" s="1">
         <v>2021</v>
       </c>
       <c r="B302" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C302" s="1">
         <v>35558</v>
@@ -7557,12 +7557,12 @@
         <v>17644</v>
       </c>
     </row>
-    <row r="303" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="303" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A303" s="1">
         <v>2021</v>
       </c>
       <c r="B303" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C303" s="1">
         <v>29303</v>
@@ -7580,12 +7580,12 @@
         <v>14594</v>
       </c>
     </row>
-    <row r="304" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="304" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A304" s="1">
         <v>2021</v>
       </c>
       <c r="B304" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C304" s="1">
         <v>7458</v>
@@ -7603,12 +7603,12 @@
         <v>3676</v>
       </c>
     </row>
-    <row r="305" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="305" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A305" s="1">
         <v>2021</v>
       </c>
       <c r="B305" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C305" s="1">
         <v>33326</v>
@@ -7626,12 +7626,12 @@
         <v>16404</v>
       </c>
     </row>
-    <row r="306" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="306" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A306" s="1">
         <v>2021</v>
       </c>
       <c r="B306" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C306" s="1">
         <v>14095</v>
@@ -7649,12 +7649,12 @@
         <v>6923</v>
       </c>
     </row>
-    <row r="307" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="307" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A307" s="1">
         <v>2021</v>
       </c>
       <c r="B307" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C307" s="1">
         <v>9089</v>
@@ -7672,12 +7672,12 @@
         <v>4431</v>
       </c>
     </row>
-    <row r="308" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="308" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A308" s="1">
         <v>2021</v>
       </c>
       <c r="B308" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C308" s="1">
         <v>5376</v>
@@ -7695,12 +7695,12 @@
         <v>2647</v>
       </c>
     </row>
-    <row r="309" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="309" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A309" s="1">
         <v>2021</v>
       </c>
       <c r="B309" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C309" s="1">
         <v>10388</v>
@@ -7718,12 +7718,12 @@
         <v>5164</v>
       </c>
     </row>
-    <row r="310" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="310" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A310" s="1">
         <v>2021</v>
       </c>
       <c r="B310" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C310" s="1">
         <v>8707</v>
@@ -7741,12 +7741,12 @@
         <v>4352</v>
       </c>
     </row>
-    <row r="311" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="311" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A311" s="1">
         <v>2021</v>
       </c>
       <c r="B311" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C311" s="1">
         <v>10170</v>
@@ -7764,12 +7764,12 @@
         <v>4900</v>
       </c>
     </row>
-    <row r="312" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="312" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A312" s="1">
         <v>2021</v>
       </c>
       <c r="B312" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C312" s="1">
         <v>328</v>
@@ -7787,12 +7787,12 @@
         <v>160</v>
       </c>
     </row>
-    <row r="313" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="313" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A313" s="1">
         <v>2021</v>
       </c>
       <c r="B313" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C313" s="1">
         <v>75</v>

</xml_diff>